<commit_message>
Commit message describing the changes
</commit_message>
<xml_diff>
--- a/wb.xlsx
+++ b/wb.xlsx
@@ -4,12 +4,25 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19620" windowHeight="8250"/>
+    <workbookView windowWidth="19635" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -104,14 +117,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Kalathi kanmoi</t>
-    </r>
+    <t>Kalathi kanmoi</t>
   </si>
   <si>
     <r>
@@ -7803,14 +7809,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Nudavembu tank</t>
-    </r>
+    <t>Nudavembu tank</t>
   </si>
   <si>
     <r>
@@ -13217,7 +13216,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
@@ -14388,8 +14387,8 @@
   <sheetPr/>
   <dimension ref="A1:H1340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" workbookViewId="0">
-      <selection activeCell="C359" sqref="C359"/>
+    <sheetView tabSelected="1" topLeftCell="A688" workbookViewId="0">
+      <selection activeCell="H696" sqref="H696"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>

</xml_diff>